<commit_message>
Includes data on amino acids
</commit_message>
<xml_diff>
--- a/MyProjects/Diet and Health/Amino acids/Data/Safe levels of protein intake.xlsx
+++ b/MyProjects/Diet and Health/Amino acids/Data/Safe levels of protein intake.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1fe936e0db66cfc0/Documents/RProjects/RProjects/MyProjects/Diet and Health/Amino acids/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="518" documentId="8_{B3C1D61D-1366-482B-92B2-30B214455D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E68DF06-E641-4806-9C3B-290CB5C2DDBA}"/>
+  <xr:revisionPtr revIDLastSave="525" documentId="8_{B3C1D61D-1366-482B-92B2-30B214455D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4A1605B-F383-4CB3-9932-EE5942FA0F43}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{A51A9851-8A88-4CB2-919E-CAFEE7296B29}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{A51A9851-8A88-4CB2-919E-CAFEE7296B29}"/>
   </bookViews>
   <sheets>
     <sheet name="safe levels" sheetId="1" r:id="rId1"/>
@@ -97,21 +97,6 @@
     <t>lactation &gt;6</t>
   </si>
   <si>
-    <t>amino acid</t>
-  </si>
-  <si>
-    <t>children (2-5 years) mg/kg/day</t>
-  </si>
-  <si>
-    <t>children (10-12 years) mg/kg/day</t>
-  </si>
-  <si>
-    <t>adults (18+ years) mg/kg/day</t>
-  </si>
-  <si>
-    <t>adults (revised) mg/kg/day</t>
-  </si>
-  <si>
     <t>isoleucine</t>
   </si>
   <si>
@@ -263,6 +248,21 @@
   </si>
   <si>
     <t>beans (pinto)</t>
+  </si>
+  <si>
+    <t>adults_revised_mg_kg_day</t>
+  </si>
+  <si>
+    <t>adults_18_years_mg_kg_day</t>
+  </si>
+  <si>
+    <t>children_10_12 years_mg_kg_day</t>
+  </si>
+  <si>
+    <t>children_2_5_years_mg_kg_day</t>
+  </si>
+  <si>
+    <t>amino_acid</t>
   </si>
 </sst>
 </file>
@@ -298,10 +298,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,9 +841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B47B98E-2E11-4F0A-ABC6-43A95407785F}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -857,24 +854,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>31</v>
@@ -891,7 +888,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>73</v>
@@ -908,7 +905,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>64</v>
@@ -925,7 +922,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>27</v>
@@ -942,7 +939,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>69</v>
@@ -959,7 +956,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>37</v>
@@ -976,7 +973,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>12.5</v>
@@ -993,7 +990,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>38</v>
@@ -1010,7 +1007,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <f>SUM(B2:B9)</f>
@@ -1038,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEE02DB-BE05-442F-BFEB-6A9213BB59BA}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
@@ -1049,45 +1046,45 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>3.5</v>
@@ -1125,7 +1122,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>17</v>
@@ -1163,7 +1160,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -1201,7 +1198,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>12.8</v>
@@ -1239,7 +1236,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>16.2</v>
@@ -1277,7 +1274,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>20.6</v>
@@ -1315,7 +1312,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>16.5</v>
@@ -1350,7 +1347,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <v>18</v>
@@ -1388,7 +1385,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>15.2</v>
@@ -1426,7 +1423,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>12.8</v>
@@ -1464,7 +1461,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -1502,7 +1499,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <v>11.4</v>
@@ -1540,7 +1537,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B14">
         <v>14.2</v>
@@ -1578,7 +1575,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>7.5</v>
@@ -1616,7 +1613,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>12.2</v>
@@ -1654,7 +1651,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>11</v>
@@ -1692,7 +1689,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B18">
         <v>14</v>
@@ -1730,7 +1727,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B19">
         <v>23</v>
@@ -1768,7 +1765,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B20">
         <v>23.1</v>
@@ -1806,7 +1803,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B21">
         <v>21.4</v>
@@ -1844,7 +1841,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B22">
         <v>25.4</v>
@@ -1882,7 +1879,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B23">
         <v>20.8</v>
@@ -1920,7 +1917,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B24">
         <v>22.9</v>
@@ -1958,7 +1955,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B25">
         <v>25</v>
@@ -1996,7 +1993,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B26">
         <v>20.7</v>
@@ -2034,7 +2031,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B27">
         <v>24.4</v>
@@ -2072,7 +2069,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>26.9</v>
@@ -2110,7 +2107,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B29">
         <v>24.5</v>
@@ -2148,7 +2145,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B30">
         <v>34.9</v>
@@ -2186,7 +2183,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B31">
         <v>3.4</v>

</xml_diff>